<commit_message>
Changes to HighF FSK, and Midterm.xlsx for filter
</commit_message>
<xml_diff>
--- a/MIDTERM.xlsx
+++ b/MIDTERM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipfajard\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPB_Data\Documents\UACSCode\UACS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -574,7 +574,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -983,7 +982,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1312,7 +1310,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7492,8 +7489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8119,7 +8116,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E56" s="1">
-        <v>220</v>
+        <v>400</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -8159,11 +8156,11 @@
       </c>
       <c r="B59" s="1">
         <f>1/(2*PI()*A59*($E$56))</f>
-        <v>7234.3155950861519</v>
+        <v>3978.8735772973832</v>
       </c>
       <c r="C59" s="1">
-        <f>B59*1.05</f>
-        <v>7596.0313748404596</v>
+        <f>B59*1.01</f>
+        <v>4018.662313070357</v>
       </c>
       <c r="E59" t="s">
         <v>79</v>
@@ -8192,11 +8189,11 @@
       </c>
       <c r="B60" s="1">
         <f t="shared" ref="B60:B63" si="11">1/(2*PI()*A60*($E$56))</f>
-        <v>72343.155950861517</v>
+        <v>39788.735772973836</v>
       </c>
       <c r="C60" s="4">
         <f t="shared" ref="C60:C63" si="12">B60*1.05</f>
-        <v>75960.313748404602</v>
+        <v>41778.17256162253</v>
       </c>
       <c r="E60" s="3">
         <v>560</v>
@@ -8225,11 +8222,11 @@
       </c>
       <c r="B61" s="1">
         <f t="shared" si="11"/>
-        <v>32883.252704937055</v>
+        <v>18085.788987715383</v>
       </c>
       <c r="C61" s="1">
         <f t="shared" si="12"/>
-        <v>34527.415340183907</v>
+        <v>18990.078437101154</v>
       </c>
       <c r="G61" s="1">
         <v>2000</v>
@@ -8255,11 +8252,11 @@
       </c>
       <c r="B62" s="1">
         <f t="shared" si="11"/>
-        <v>15392.160840608833</v>
+        <v>8465.6884623348578</v>
       </c>
       <c r="C62" s="1">
         <f t="shared" si="12"/>
-        <v>16161.768882639275</v>
+        <v>8888.9728854516015</v>
       </c>
       <c r="G62" s="2">
         <v>2200</v>
@@ -8285,11 +8282,11 @@
       </c>
       <c r="B63" s="1">
         <f t="shared" si="11"/>
-        <v>72.343155950861515</v>
+        <v>39.78873577297383</v>
       </c>
       <c r="C63" s="1">
         <f t="shared" si="12"/>
-        <v>75.960313748404587</v>
+        <v>41.778172561622526</v>
       </c>
       <c r="G63" s="1">
         <v>4700</v>

</xml_diff>